<commit_message>
Latest code update on 22th April
</commit_message>
<xml_diff>
--- a/ExcelDataDriven/Data/Book1.xlsx
+++ b/ExcelDataDriven/Data/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShanikaHettiarachchi\eclipse-workspace\ExcelDataDriven\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC65A8FC-8E46-45B5-B0F4-5D1E2CB585EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E764CC95-54AD-485D-98B7-D93B81FA947C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="7965" xr2:uid="{AD57807F-FC20-4237-98D4-6ABA4D43B6E4}"/>
+    <workbookView xWindow="31005" yWindow="1995" windowWidth="15375" windowHeight="7965" xr2:uid="{AD57807F-FC20-4237-98D4-6ABA4D43B6E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,22 +35,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>URL</t>
   </si>
   <si>
     <t>https://demo.guru99.com/insurance/v1/index.php</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>F_Name</t>
+  </si>
+  <si>
+    <t>L_Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>B_Year</t>
+  </si>
+  <si>
+    <t>B_Month</t>
+  </si>
+  <si>
+    <t>B_Date</t>
+  </si>
+  <si>
+    <t>Shani</t>
+  </si>
+  <si>
+    <t>Hettiarachchi</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>L_Type</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>L_Period</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Street_Add</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Counrty</t>
+  </si>
+  <si>
+    <t>Post_Code</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm_Password</t>
+  </si>
+  <si>
+    <t>146/6A</t>
+  </si>
+  <si>
+    <t>Piliyandala</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>hettiarachchism@gmail.com</t>
+  </si>
+  <si>
+    <t>Shani@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,13 +172,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,25 +497,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487D634D-18C2-446B-82BB-4E2326EAF1F7}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>718400116</v>
+      </c>
+      <c r="F2">
+        <v>1988</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>10300</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{4246884F-1834-4D8B-9E8B-9BC12E2A4A86}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{73E630BE-40BD-4EA7-9333-C172829A6FC3}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{61BEB885-3255-48CB-AEA3-3AD1F6095632}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ExcelDataDriven TestNG Matrix reports
</commit_message>
<xml_diff>
--- a/ExcelDataDriven/Data/Book1.xlsx
+++ b/ExcelDataDriven/Data/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShanikaHettiarachchi\eclipse-workspace\ExcelDataDriven\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E764CC95-54AD-485D-98B7-D93B81FA947C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138715F5-91CC-40AF-8830-92F94F93CF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31005" yWindow="1995" windowWidth="15375" windowHeight="7965" xr2:uid="{AD57807F-FC20-4237-98D4-6ABA4D43B6E4}"/>
+    <workbookView xWindow="3735" yWindow="1680" windowWidth="15375" windowHeight="7965" xr2:uid="{AD57807F-FC20-4237-98D4-6ABA4D43B6E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>